<commit_message>
PPE-105234 : Modified tests to handle qa02 as perf (Sub Tasks : PPE-118033, PPE-118034)
</commit_message>
<xml_diff>
--- a/test/pb2/fe/jira/release29/ppe-105234/qa00_bulkimport.xlsx
+++ b/test/pb2/fe/jira/release29/ppe-105234/qa00_bulkimport.xlsx
@@ -24,16 +24,16 @@
     <t>to</t>
   </si>
   <si>
-    <t>http://www.qa00.webmd.com/fitness-exercise/features/tired-of-exercise</t>
-  </si>
-  <si>
-    <t>http://www.qa00.webmd.com/men/stick-with-fitness-plan</t>
-  </si>
-  <si>
     <t>http://www.qa00.webmd.com/fitness-exercise/features/tired-of-exercise/testingpurpose/2019/6</t>
   </si>
   <si>
     <t>http://www.qa00.webmd.com/men/stick-with-fitness-plan/testingpurpose/2019/6</t>
+  </si>
+  <si>
+    <t>http://www.qa00.webmd.com/fitness-exercise/features/tired-of-exercise/testingpurpose</t>
+  </si>
+  <si>
+    <t>http://www.qa00.webmd.com/men/stick-with-fitness-plan/testingpurpose</t>
   </si>
 </sst>
 </file>
@@ -878,7 +878,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,19 +896,19 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -947,6 +947,8 @@
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="http://www.dev03.webmd.com/fitness-exercise/features/tired-of-exercise/testingpurpose/2019/6"/>
     <hyperlink ref="B3" r:id="rId2" display="http://www.dev03.webmd.com/men/stick-with-fitness-plan/testingpurpose/2019/6"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>